<commit_message>
Dude looks like a lady
</commit_message>
<xml_diff>
--- a/assets/uploads/Factura Lunes.xlsx
+++ b/assets/uploads/Factura Lunes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>CÓDIGO PROVEEDOR</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>FECHA EN LA FACTURA</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN</t>
   </si>
 </sst>
 </file>
@@ -409,41 +412,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="3"/>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>